<commit_message>
more expression working, but need to use AST??
</commit_message>
<xml_diff>
--- a/doc/design-note.xlsx
+++ b/doc/design-note.xlsx
@@ -26,7 +26,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="120" uniqueCount="74">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="182" uniqueCount="94">
   <si>
     <t>code block</t>
   </si>
@@ -232,22 +232,82 @@
     <t>;</t>
   </si>
   <si>
-    <t xml:space="preserve">  ret =  &lt;primary_expression_0&gt; aaa  &lt;primary_expression_0&gt; * bbb  &lt;primary_expression_0&gt; /  &lt;multipricative_expression_1&gt; </t>
-  </si>
-  <si>
-    <t xml:space="preserve">  ( aaa  &lt;primary_expression_0&gt; + bbb  &lt;primary_expression_0&gt; +  &lt;additive_expression_1&gt; 100  &lt;primary_expression_1&gt; </t>
-  </si>
-  <si>
-    <t xml:space="preserve">  / aaa  &lt;primary_expression_0&gt; )  &lt;multipricative_expression_2&gt;  &lt;additive_expression_1&gt;  &lt;primary_expression_3&gt; /  </t>
-  </si>
-  <si>
-    <t xml:space="preserve">  &lt;multipricative_expression_2&gt; ( ( unsigned char ) bbb  &lt;primary_expression_0&gt; %  &lt;cast_expression_1&gt; aaa  &lt;primary_expression_0&gt; )  </t>
-  </si>
-  <si>
-    <t xml:space="preserve">  &lt;multipricative_expression_3&gt;  &lt;primary_expression_3&gt; ;</t>
-  </si>
-  <si>
-    <t xml:space="preserve"> &lt;multipricative_expression_2&gt;  &lt;assignment_expression_1&gt;   return ret  &lt;primary_expression_0&gt; ;</t>
+    <t xml:space="preserve">  ret =  &lt;1. primary_expression_0&gt; aaa  &lt;2. primary_expression_0&gt; * bbb  &lt;3. primary_expression_0&gt; /  &lt;4. multipricative_expression_1&gt; </t>
+  </si>
+  <si>
+    <t xml:space="preserve">  ( aaa  &lt;5. primary_expression_0&gt; + bbb  &lt;6. primary_expression_0&gt; +  &lt;7. additive_expression_1&gt; 100  &lt;8. primary_expression_1&gt; </t>
+  </si>
+  <si>
+    <t xml:space="preserve">  / aaa  &lt;9. primary_expression_0&gt; )  &lt;10. multipricative_expression_2&gt;  &lt;11. additive_expression_1&gt;  &lt;12. primary_expression_3&gt; /  </t>
+  </si>
+  <si>
+    <t xml:space="preserve">  &lt;13. multipricative_expression_2&gt; ( ( unsigned char ) bbb  &lt;14. primary_expression_0&gt; %  &lt;15. cast_expression_1&gt; aaa  &lt;16. primary_expression_0&gt; )  </t>
+  </si>
+  <si>
+    <t xml:space="preserve">  &lt;17. multipricative_expression_3&gt;  &lt;18. primary_expression_3&gt; ;</t>
+  </si>
+  <si>
+    <t xml:space="preserve"> &lt;19. multipricative_expression_2&gt;  &lt;20. assignment_expression_1&gt; </t>
+  </si>
+  <si>
+    <t>stack</t>
+  </si>
+  <si>
+    <t>ret</t>
+  </si>
+  <si>
+    <t>=</t>
+  </si>
+  <si>
+    <t>bbb</t>
+  </si>
+  <si>
+    <t>exp1</t>
+  </si>
+  <si>
+    <t>exp2</t>
+  </si>
+  <si>
+    <t>*</t>
+  </si>
+  <si>
+    <t>/</t>
+  </si>
+  <si>
+    <t>+</t>
+  </si>
+  <si>
+    <t>exp3</t>
+  </si>
+  <si>
+    <t>exp4</t>
+  </si>
+  <si>
+    <t>exp5</t>
+  </si>
+  <si>
+    <t>exp6</t>
+  </si>
+  <si>
+    <t>unsigned</t>
+  </si>
+  <si>
+    <t>%</t>
+  </si>
+  <si>
+    <t>exp7</t>
+  </si>
+  <si>
+    <t>exp8</t>
+  </si>
+  <si>
+    <t>exp9</t>
+  </si>
+  <si>
+    <t>exp10</t>
+  </si>
+  <si>
+    <t>exp11</t>
   </si>
 </sst>
 </file>
@@ -264,12 +324,18 @@
       <scheme val="minor"/>
     </font>
   </fonts>
-  <fills count="2">
+  <fills count="3">
     <fill>
       <patternFill patternType="none"/>
     </fill>
     <fill>
       <patternFill patternType="gray125"/>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FFFFFF00"/>
+        <bgColor indexed="64"/>
+      </patternFill>
     </fill>
   </fills>
   <borders count="1">
@@ -284,11 +350,13 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="2">
+  <cellXfs count="4">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
-      <alignment horizontal="left"/>
+      <alignment horizontal="center"/>
     </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" quotePrefix="1"/>
+    <xf numFmtId="0" fontId="0" fillId="2" borderId="0" xfId="0" applyFill="1"/>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -601,6 +669,1051 @@
 </xdr:wsDr>
 </file>
 
+<file path=xl/drawings/drawing2.xml><?xml version="1.0" encoding="utf-8"?>
+<xdr:wsDr xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main">
+  <xdr:twoCellAnchor>
+    <xdr:from>
+      <xdr:col>1</xdr:col>
+      <xdr:colOff>28575</xdr:colOff>
+      <xdr:row>15</xdr:row>
+      <xdr:rowOff>38100</xdr:rowOff>
+    </xdr:from>
+    <xdr:to>
+      <xdr:col>1</xdr:col>
+      <xdr:colOff>352425</xdr:colOff>
+      <xdr:row>16</xdr:row>
+      <xdr:rowOff>19050</xdr:rowOff>
+    </xdr:to>
+    <xdr:sp macro="" textlink="">
+      <xdr:nvSpPr>
+        <xdr:cNvPr id="3" name="Left Bracket 2"/>
+        <xdr:cNvSpPr/>
+      </xdr:nvSpPr>
+      <xdr:spPr>
+        <a:xfrm rot="16200000">
+          <a:off x="714375" y="2819400"/>
+          <a:ext cx="171450" cy="323850"/>
+        </a:xfrm>
+        <a:prstGeom prst="leftBracket">
+          <a:avLst/>
+        </a:prstGeom>
+      </xdr:spPr>
+      <xdr:style>
+        <a:lnRef idx="3">
+          <a:schemeClr val="dk1"/>
+        </a:lnRef>
+        <a:fillRef idx="0">
+          <a:schemeClr val="dk1"/>
+        </a:fillRef>
+        <a:effectRef idx="2">
+          <a:schemeClr val="dk1"/>
+        </a:effectRef>
+        <a:fontRef idx="minor">
+          <a:schemeClr val="tx1"/>
+        </a:fontRef>
+      </xdr:style>
+      <xdr:txBody>
+        <a:bodyPr vertOverflow="clip" horzOverflow="clip" rtlCol="0" anchor="t"/>
+        <a:lstStyle/>
+        <a:p>
+          <a:pPr algn="l"/>
+          <a:endParaRPr lang="en-GB" sz="1100"/>
+        </a:p>
+      </xdr:txBody>
+    </xdr:sp>
+    <xdr:clientData/>
+  </xdr:twoCellAnchor>
+  <xdr:twoCellAnchor>
+    <xdr:from>
+      <xdr:col>3</xdr:col>
+      <xdr:colOff>19050</xdr:colOff>
+      <xdr:row>15</xdr:row>
+      <xdr:rowOff>38100</xdr:rowOff>
+    </xdr:from>
+    <xdr:to>
+      <xdr:col>3</xdr:col>
+      <xdr:colOff>342900</xdr:colOff>
+      <xdr:row>16</xdr:row>
+      <xdr:rowOff>19050</xdr:rowOff>
+    </xdr:to>
+    <xdr:sp macro="" textlink="">
+      <xdr:nvSpPr>
+        <xdr:cNvPr id="4" name="Left Bracket 3"/>
+        <xdr:cNvSpPr/>
+      </xdr:nvSpPr>
+      <xdr:spPr>
+        <a:xfrm rot="16200000">
+          <a:off x="1447800" y="2819400"/>
+          <a:ext cx="171450" cy="323850"/>
+        </a:xfrm>
+        <a:prstGeom prst="leftBracket">
+          <a:avLst/>
+        </a:prstGeom>
+      </xdr:spPr>
+      <xdr:style>
+        <a:lnRef idx="3">
+          <a:schemeClr val="dk1"/>
+        </a:lnRef>
+        <a:fillRef idx="0">
+          <a:schemeClr val="dk1"/>
+        </a:fillRef>
+        <a:effectRef idx="2">
+          <a:schemeClr val="dk1"/>
+        </a:effectRef>
+        <a:fontRef idx="minor">
+          <a:schemeClr val="tx1"/>
+        </a:fontRef>
+      </xdr:style>
+      <xdr:txBody>
+        <a:bodyPr vertOverflow="clip" horzOverflow="clip" rtlCol="0" anchor="t"/>
+        <a:lstStyle/>
+        <a:p>
+          <a:pPr algn="l"/>
+          <a:endParaRPr lang="en-GB" sz="1100"/>
+        </a:p>
+      </xdr:txBody>
+    </xdr:sp>
+    <xdr:clientData/>
+  </xdr:twoCellAnchor>
+  <xdr:twoCellAnchor>
+    <xdr:from>
+      <xdr:col>4</xdr:col>
+      <xdr:colOff>361950</xdr:colOff>
+      <xdr:row>15</xdr:row>
+      <xdr:rowOff>66675</xdr:rowOff>
+    </xdr:from>
+    <xdr:to>
+      <xdr:col>5</xdr:col>
+      <xdr:colOff>314325</xdr:colOff>
+      <xdr:row>16</xdr:row>
+      <xdr:rowOff>47625</xdr:rowOff>
+    </xdr:to>
+    <xdr:sp macro="" textlink="">
+      <xdr:nvSpPr>
+        <xdr:cNvPr id="5" name="Left Bracket 4"/>
+        <xdr:cNvSpPr/>
+      </xdr:nvSpPr>
+      <xdr:spPr>
+        <a:xfrm rot="16200000">
+          <a:off x="2162175" y="2847975"/>
+          <a:ext cx="171450" cy="323850"/>
+        </a:xfrm>
+        <a:prstGeom prst="leftBracket">
+          <a:avLst/>
+        </a:prstGeom>
+      </xdr:spPr>
+      <xdr:style>
+        <a:lnRef idx="3">
+          <a:schemeClr val="dk1"/>
+        </a:lnRef>
+        <a:fillRef idx="0">
+          <a:schemeClr val="dk1"/>
+        </a:fillRef>
+        <a:effectRef idx="2">
+          <a:schemeClr val="dk1"/>
+        </a:effectRef>
+        <a:fontRef idx="minor">
+          <a:schemeClr val="tx1"/>
+        </a:fontRef>
+      </xdr:style>
+      <xdr:txBody>
+        <a:bodyPr vertOverflow="clip" horzOverflow="clip" rtlCol="0" anchor="t"/>
+        <a:lstStyle/>
+        <a:p>
+          <a:pPr algn="l"/>
+          <a:endParaRPr lang="en-GB" sz="1100"/>
+        </a:p>
+      </xdr:txBody>
+    </xdr:sp>
+    <xdr:clientData/>
+  </xdr:twoCellAnchor>
+  <xdr:twoCellAnchor>
+    <xdr:from>
+      <xdr:col>3</xdr:col>
+      <xdr:colOff>28574</xdr:colOff>
+      <xdr:row>17</xdr:row>
+      <xdr:rowOff>0</xdr:rowOff>
+    </xdr:from>
+    <xdr:to>
+      <xdr:col>5</xdr:col>
+      <xdr:colOff>304799</xdr:colOff>
+      <xdr:row>17</xdr:row>
+      <xdr:rowOff>161925</xdr:rowOff>
+    </xdr:to>
+    <xdr:sp macro="" textlink="">
+      <xdr:nvSpPr>
+        <xdr:cNvPr id="6" name="Left Bracket 5"/>
+        <xdr:cNvSpPr/>
+      </xdr:nvSpPr>
+      <xdr:spPr>
+        <a:xfrm rot="16200000">
+          <a:off x="1809749" y="2809875"/>
+          <a:ext cx="161925" cy="1019175"/>
+        </a:xfrm>
+        <a:prstGeom prst="leftBracket">
+          <a:avLst/>
+        </a:prstGeom>
+      </xdr:spPr>
+      <xdr:style>
+        <a:lnRef idx="3">
+          <a:schemeClr val="dk1"/>
+        </a:lnRef>
+        <a:fillRef idx="0">
+          <a:schemeClr val="dk1"/>
+        </a:fillRef>
+        <a:effectRef idx="2">
+          <a:schemeClr val="dk1"/>
+        </a:effectRef>
+        <a:fontRef idx="minor">
+          <a:schemeClr val="tx1"/>
+        </a:fontRef>
+      </xdr:style>
+      <xdr:txBody>
+        <a:bodyPr vertOverflow="clip" horzOverflow="clip" rtlCol="0" anchor="t"/>
+        <a:lstStyle/>
+        <a:p>
+          <a:pPr algn="l"/>
+          <a:endParaRPr lang="en-GB" sz="1100"/>
+        </a:p>
+      </xdr:txBody>
+    </xdr:sp>
+    <xdr:clientData/>
+  </xdr:twoCellAnchor>
+  <xdr:twoCellAnchor>
+    <xdr:from>
+      <xdr:col>8</xdr:col>
+      <xdr:colOff>47625</xdr:colOff>
+      <xdr:row>17</xdr:row>
+      <xdr:rowOff>28575</xdr:rowOff>
+    </xdr:from>
+    <xdr:to>
+      <xdr:col>9</xdr:col>
+      <xdr:colOff>0</xdr:colOff>
+      <xdr:row>18</xdr:row>
+      <xdr:rowOff>9525</xdr:rowOff>
+    </xdr:to>
+    <xdr:sp macro="" textlink="">
+      <xdr:nvSpPr>
+        <xdr:cNvPr id="7" name="Left Bracket 6"/>
+        <xdr:cNvSpPr/>
+      </xdr:nvSpPr>
+      <xdr:spPr>
+        <a:xfrm rot="16200000">
+          <a:off x="3333750" y="3190875"/>
+          <a:ext cx="171450" cy="323850"/>
+        </a:xfrm>
+        <a:prstGeom prst="leftBracket">
+          <a:avLst/>
+        </a:prstGeom>
+      </xdr:spPr>
+      <xdr:style>
+        <a:lnRef idx="3">
+          <a:schemeClr val="dk1"/>
+        </a:lnRef>
+        <a:fillRef idx="0">
+          <a:schemeClr val="dk1"/>
+        </a:fillRef>
+        <a:effectRef idx="2">
+          <a:schemeClr val="dk1"/>
+        </a:effectRef>
+        <a:fontRef idx="minor">
+          <a:schemeClr val="tx1"/>
+        </a:fontRef>
+      </xdr:style>
+      <xdr:txBody>
+        <a:bodyPr vertOverflow="clip" horzOverflow="clip" rtlCol="0" anchor="t"/>
+        <a:lstStyle/>
+        <a:p>
+          <a:pPr algn="l"/>
+          <a:endParaRPr lang="en-GB" sz="1100"/>
+        </a:p>
+      </xdr:txBody>
+    </xdr:sp>
+    <xdr:clientData/>
+  </xdr:twoCellAnchor>
+  <xdr:twoCellAnchor>
+    <xdr:from>
+      <xdr:col>10</xdr:col>
+      <xdr:colOff>47625</xdr:colOff>
+      <xdr:row>17</xdr:row>
+      <xdr:rowOff>9525</xdr:rowOff>
+    </xdr:from>
+    <xdr:to>
+      <xdr:col>11</xdr:col>
+      <xdr:colOff>0</xdr:colOff>
+      <xdr:row>17</xdr:row>
+      <xdr:rowOff>180975</xdr:rowOff>
+    </xdr:to>
+    <xdr:sp macro="" textlink="">
+      <xdr:nvSpPr>
+        <xdr:cNvPr id="8" name="Left Bracket 7"/>
+        <xdr:cNvSpPr/>
+      </xdr:nvSpPr>
+      <xdr:spPr>
+        <a:xfrm rot="16200000">
+          <a:off x="4076700" y="3171825"/>
+          <a:ext cx="171450" cy="323850"/>
+        </a:xfrm>
+        <a:prstGeom prst="leftBracket">
+          <a:avLst/>
+        </a:prstGeom>
+      </xdr:spPr>
+      <xdr:style>
+        <a:lnRef idx="3">
+          <a:schemeClr val="dk1"/>
+        </a:lnRef>
+        <a:fillRef idx="0">
+          <a:schemeClr val="dk1"/>
+        </a:fillRef>
+        <a:effectRef idx="2">
+          <a:schemeClr val="dk1"/>
+        </a:effectRef>
+        <a:fontRef idx="minor">
+          <a:schemeClr val="tx1"/>
+        </a:fontRef>
+      </xdr:style>
+      <xdr:txBody>
+        <a:bodyPr vertOverflow="clip" horzOverflow="clip" rtlCol="0" anchor="t"/>
+        <a:lstStyle/>
+        <a:p>
+          <a:pPr algn="l"/>
+          <a:endParaRPr lang="en-GB" sz="1100"/>
+        </a:p>
+      </xdr:txBody>
+    </xdr:sp>
+    <xdr:clientData/>
+  </xdr:twoCellAnchor>
+  <xdr:twoCellAnchor>
+    <xdr:from>
+      <xdr:col>12</xdr:col>
+      <xdr:colOff>28575</xdr:colOff>
+      <xdr:row>21</xdr:row>
+      <xdr:rowOff>9525</xdr:rowOff>
+    </xdr:from>
+    <xdr:to>
+      <xdr:col>14</xdr:col>
+      <xdr:colOff>304800</xdr:colOff>
+      <xdr:row>21</xdr:row>
+      <xdr:rowOff>171450</xdr:rowOff>
+    </xdr:to>
+    <xdr:sp macro="" textlink="">
+      <xdr:nvSpPr>
+        <xdr:cNvPr id="10" name="Left Bracket 9"/>
+        <xdr:cNvSpPr/>
+      </xdr:nvSpPr>
+      <xdr:spPr>
+        <a:xfrm rot="16200000">
+          <a:off x="5153025" y="3581400"/>
+          <a:ext cx="161925" cy="1019175"/>
+        </a:xfrm>
+        <a:prstGeom prst="leftBracket">
+          <a:avLst/>
+        </a:prstGeom>
+      </xdr:spPr>
+      <xdr:style>
+        <a:lnRef idx="3">
+          <a:schemeClr val="dk1"/>
+        </a:lnRef>
+        <a:fillRef idx="0">
+          <a:schemeClr val="dk1"/>
+        </a:fillRef>
+        <a:effectRef idx="2">
+          <a:schemeClr val="dk1"/>
+        </a:effectRef>
+        <a:fontRef idx="minor">
+          <a:schemeClr val="tx1"/>
+        </a:fontRef>
+      </xdr:style>
+      <xdr:txBody>
+        <a:bodyPr vertOverflow="clip" horzOverflow="clip" rtlCol="0" anchor="t"/>
+        <a:lstStyle/>
+        <a:p>
+          <a:pPr algn="l"/>
+          <a:endParaRPr lang="en-GB" sz="1100"/>
+        </a:p>
+      </xdr:txBody>
+    </xdr:sp>
+    <xdr:clientData/>
+  </xdr:twoCellAnchor>
+  <xdr:twoCellAnchor>
+    <xdr:from>
+      <xdr:col>12</xdr:col>
+      <xdr:colOff>0</xdr:colOff>
+      <xdr:row>19</xdr:row>
+      <xdr:rowOff>9525</xdr:rowOff>
+    </xdr:from>
+    <xdr:to>
+      <xdr:col>12</xdr:col>
+      <xdr:colOff>323850</xdr:colOff>
+      <xdr:row>19</xdr:row>
+      <xdr:rowOff>180975</xdr:rowOff>
+    </xdr:to>
+    <xdr:sp macro="" textlink="">
+      <xdr:nvSpPr>
+        <xdr:cNvPr id="11" name="Left Bracket 10"/>
+        <xdr:cNvSpPr/>
+      </xdr:nvSpPr>
+      <xdr:spPr>
+        <a:xfrm rot="16200000">
+          <a:off x="4772025" y="3552825"/>
+          <a:ext cx="171450" cy="323850"/>
+        </a:xfrm>
+        <a:prstGeom prst="leftBracket">
+          <a:avLst/>
+        </a:prstGeom>
+      </xdr:spPr>
+      <xdr:style>
+        <a:lnRef idx="3">
+          <a:schemeClr val="dk1"/>
+        </a:lnRef>
+        <a:fillRef idx="0">
+          <a:schemeClr val="dk1"/>
+        </a:fillRef>
+        <a:effectRef idx="2">
+          <a:schemeClr val="dk1"/>
+        </a:effectRef>
+        <a:fontRef idx="minor">
+          <a:schemeClr val="tx1"/>
+        </a:fontRef>
+      </xdr:style>
+      <xdr:txBody>
+        <a:bodyPr vertOverflow="clip" horzOverflow="clip" rtlCol="0" anchor="t"/>
+        <a:lstStyle/>
+        <a:p>
+          <a:pPr algn="l"/>
+          <a:endParaRPr lang="en-GB" sz="1100"/>
+        </a:p>
+      </xdr:txBody>
+    </xdr:sp>
+    <xdr:clientData/>
+  </xdr:twoCellAnchor>
+  <xdr:twoCellAnchor>
+    <xdr:from>
+      <xdr:col>14</xdr:col>
+      <xdr:colOff>0</xdr:colOff>
+      <xdr:row>19</xdr:row>
+      <xdr:rowOff>0</xdr:rowOff>
+    </xdr:from>
+    <xdr:to>
+      <xdr:col>14</xdr:col>
+      <xdr:colOff>323850</xdr:colOff>
+      <xdr:row>19</xdr:row>
+      <xdr:rowOff>171450</xdr:rowOff>
+    </xdr:to>
+    <xdr:sp macro="" textlink="">
+      <xdr:nvSpPr>
+        <xdr:cNvPr id="12" name="Left Bracket 11"/>
+        <xdr:cNvSpPr/>
+      </xdr:nvSpPr>
+      <xdr:spPr>
+        <a:xfrm rot="16200000">
+          <a:off x="5514975" y="3543300"/>
+          <a:ext cx="171450" cy="323850"/>
+        </a:xfrm>
+        <a:prstGeom prst="leftBracket">
+          <a:avLst/>
+        </a:prstGeom>
+      </xdr:spPr>
+      <xdr:style>
+        <a:lnRef idx="3">
+          <a:schemeClr val="dk1"/>
+        </a:lnRef>
+        <a:fillRef idx="0">
+          <a:schemeClr val="dk1"/>
+        </a:fillRef>
+        <a:effectRef idx="2">
+          <a:schemeClr val="dk1"/>
+        </a:effectRef>
+        <a:fontRef idx="minor">
+          <a:schemeClr val="tx1"/>
+        </a:fontRef>
+      </xdr:style>
+      <xdr:txBody>
+        <a:bodyPr vertOverflow="clip" horzOverflow="clip" rtlCol="0" anchor="t"/>
+        <a:lstStyle/>
+        <a:p>
+          <a:pPr algn="l"/>
+          <a:endParaRPr lang="en-GB" sz="1100"/>
+        </a:p>
+      </xdr:txBody>
+    </xdr:sp>
+    <xdr:clientData/>
+  </xdr:twoCellAnchor>
+  <xdr:twoCellAnchor>
+    <xdr:from>
+      <xdr:col>8</xdr:col>
+      <xdr:colOff>28575</xdr:colOff>
+      <xdr:row>19</xdr:row>
+      <xdr:rowOff>66675</xdr:rowOff>
+    </xdr:from>
+    <xdr:to>
+      <xdr:col>10</xdr:col>
+      <xdr:colOff>304800</xdr:colOff>
+      <xdr:row>20</xdr:row>
+      <xdr:rowOff>38100</xdr:rowOff>
+    </xdr:to>
+    <xdr:sp macro="" textlink="">
+      <xdr:nvSpPr>
+        <xdr:cNvPr id="13" name="Left Bracket 12"/>
+        <xdr:cNvSpPr/>
+      </xdr:nvSpPr>
+      <xdr:spPr>
+        <a:xfrm rot="16200000">
+          <a:off x="3667125" y="3257550"/>
+          <a:ext cx="161925" cy="1019175"/>
+        </a:xfrm>
+        <a:prstGeom prst="leftBracket">
+          <a:avLst/>
+        </a:prstGeom>
+      </xdr:spPr>
+      <xdr:style>
+        <a:lnRef idx="3">
+          <a:schemeClr val="dk1"/>
+        </a:lnRef>
+        <a:fillRef idx="0">
+          <a:schemeClr val="dk1"/>
+        </a:fillRef>
+        <a:effectRef idx="2">
+          <a:schemeClr val="dk1"/>
+        </a:effectRef>
+        <a:fontRef idx="minor">
+          <a:schemeClr val="tx1"/>
+        </a:fontRef>
+      </xdr:style>
+      <xdr:txBody>
+        <a:bodyPr vertOverflow="clip" horzOverflow="clip" rtlCol="0" anchor="t"/>
+        <a:lstStyle/>
+        <a:p>
+          <a:pPr algn="l"/>
+          <a:endParaRPr lang="en-GB" sz="1100"/>
+        </a:p>
+      </xdr:txBody>
+    </xdr:sp>
+    <xdr:clientData/>
+  </xdr:twoCellAnchor>
+  <xdr:twoCellAnchor>
+    <xdr:from>
+      <xdr:col>8</xdr:col>
+      <xdr:colOff>47625</xdr:colOff>
+      <xdr:row>23</xdr:row>
+      <xdr:rowOff>19049</xdr:rowOff>
+    </xdr:from>
+    <xdr:to>
+      <xdr:col>14</xdr:col>
+      <xdr:colOff>361950</xdr:colOff>
+      <xdr:row>24</xdr:row>
+      <xdr:rowOff>9524</xdr:rowOff>
+    </xdr:to>
+    <xdr:sp macro="" textlink="">
+      <xdr:nvSpPr>
+        <xdr:cNvPr id="14" name="Left Bracket 13"/>
+        <xdr:cNvSpPr/>
+      </xdr:nvSpPr>
+      <xdr:spPr>
+        <a:xfrm rot="16200000">
+          <a:off x="4438650" y="3219449"/>
+          <a:ext cx="180975" cy="2543175"/>
+        </a:xfrm>
+        <a:prstGeom prst="leftBracket">
+          <a:avLst/>
+        </a:prstGeom>
+      </xdr:spPr>
+      <xdr:style>
+        <a:lnRef idx="3">
+          <a:schemeClr val="dk1"/>
+        </a:lnRef>
+        <a:fillRef idx="0">
+          <a:schemeClr val="dk1"/>
+        </a:fillRef>
+        <a:effectRef idx="2">
+          <a:schemeClr val="dk1"/>
+        </a:effectRef>
+        <a:fontRef idx="minor">
+          <a:schemeClr val="tx1"/>
+        </a:fontRef>
+      </xdr:style>
+      <xdr:txBody>
+        <a:bodyPr vertOverflow="clip" horzOverflow="clip" rtlCol="0" anchor="t"/>
+        <a:lstStyle/>
+        <a:p>
+          <a:pPr algn="l"/>
+          <a:endParaRPr lang="en-GB" sz="1100"/>
+        </a:p>
+      </xdr:txBody>
+    </xdr:sp>
+    <xdr:clientData/>
+  </xdr:twoCellAnchor>
+  <xdr:twoCellAnchor>
+    <xdr:from>
+      <xdr:col>7</xdr:col>
+      <xdr:colOff>57150</xdr:colOff>
+      <xdr:row>25</xdr:row>
+      <xdr:rowOff>19048</xdr:rowOff>
+    </xdr:from>
+    <xdr:to>
+      <xdr:col>15</xdr:col>
+      <xdr:colOff>361950</xdr:colOff>
+      <xdr:row>26</xdr:row>
+      <xdr:rowOff>9524</xdr:rowOff>
+    </xdr:to>
+    <xdr:sp macro="" textlink="">
+      <xdr:nvSpPr>
+        <xdr:cNvPr id="15" name="Left Bracket 14"/>
+        <xdr:cNvSpPr/>
+      </xdr:nvSpPr>
+      <xdr:spPr>
+        <a:xfrm rot="16200000">
+          <a:off x="4443412" y="3233736"/>
+          <a:ext cx="180976" cy="3276600"/>
+        </a:xfrm>
+        <a:prstGeom prst="leftBracket">
+          <a:avLst/>
+        </a:prstGeom>
+      </xdr:spPr>
+      <xdr:style>
+        <a:lnRef idx="3">
+          <a:schemeClr val="dk1"/>
+        </a:lnRef>
+        <a:fillRef idx="0">
+          <a:schemeClr val="dk1"/>
+        </a:fillRef>
+        <a:effectRef idx="2">
+          <a:schemeClr val="dk1"/>
+        </a:effectRef>
+        <a:fontRef idx="minor">
+          <a:schemeClr val="tx1"/>
+        </a:fontRef>
+      </xdr:style>
+      <xdr:txBody>
+        <a:bodyPr vertOverflow="clip" horzOverflow="clip" rtlCol="0" anchor="t"/>
+        <a:lstStyle/>
+        <a:p>
+          <a:pPr algn="l"/>
+          <a:endParaRPr lang="en-GB" sz="1100"/>
+        </a:p>
+      </xdr:txBody>
+    </xdr:sp>
+    <xdr:clientData/>
+  </xdr:twoCellAnchor>
+  <xdr:twoCellAnchor>
+    <xdr:from>
+      <xdr:col>2</xdr:col>
+      <xdr:colOff>361950</xdr:colOff>
+      <xdr:row>27</xdr:row>
+      <xdr:rowOff>9522</xdr:rowOff>
+    </xdr:from>
+    <xdr:to>
+      <xdr:col>16</xdr:col>
+      <xdr:colOff>19050</xdr:colOff>
+      <xdr:row>27</xdr:row>
+      <xdr:rowOff>190499</xdr:rowOff>
+    </xdr:to>
+    <xdr:sp macro="" textlink="">
+      <xdr:nvSpPr>
+        <xdr:cNvPr id="16" name="Left Bracket 15"/>
+        <xdr:cNvSpPr/>
+      </xdr:nvSpPr>
+      <xdr:spPr>
+        <a:xfrm rot="16200000">
+          <a:off x="3681411" y="2814636"/>
+          <a:ext cx="180977" cy="4857750"/>
+        </a:xfrm>
+        <a:prstGeom prst="leftBracket">
+          <a:avLst/>
+        </a:prstGeom>
+      </xdr:spPr>
+      <xdr:style>
+        <a:lnRef idx="3">
+          <a:schemeClr val="dk1"/>
+        </a:lnRef>
+        <a:fillRef idx="0">
+          <a:schemeClr val="dk1"/>
+        </a:fillRef>
+        <a:effectRef idx="2">
+          <a:schemeClr val="dk1"/>
+        </a:effectRef>
+        <a:fontRef idx="minor">
+          <a:schemeClr val="tx1"/>
+        </a:fontRef>
+      </xdr:style>
+      <xdr:txBody>
+        <a:bodyPr vertOverflow="clip" horzOverflow="clip" rtlCol="0" anchor="t"/>
+        <a:lstStyle/>
+        <a:p>
+          <a:pPr algn="l"/>
+          <a:endParaRPr lang="en-GB" sz="1100"/>
+        </a:p>
+      </xdr:txBody>
+    </xdr:sp>
+    <xdr:clientData/>
+  </xdr:twoCellAnchor>
+  <xdr:twoCellAnchor>
+    <xdr:from>
+      <xdr:col>22</xdr:col>
+      <xdr:colOff>19050</xdr:colOff>
+      <xdr:row>27</xdr:row>
+      <xdr:rowOff>47625</xdr:rowOff>
+    </xdr:from>
+    <xdr:to>
+      <xdr:col>22</xdr:col>
+      <xdr:colOff>342900</xdr:colOff>
+      <xdr:row>28</xdr:row>
+      <xdr:rowOff>28575</xdr:rowOff>
+    </xdr:to>
+    <xdr:sp macro="" textlink="">
+      <xdr:nvSpPr>
+        <xdr:cNvPr id="17" name="Left Bracket 16"/>
+        <xdr:cNvSpPr/>
+      </xdr:nvSpPr>
+      <xdr:spPr>
+        <a:xfrm rot="16200000">
+          <a:off x="8772525" y="5114925"/>
+          <a:ext cx="171450" cy="323850"/>
+        </a:xfrm>
+        <a:prstGeom prst="leftBracket">
+          <a:avLst/>
+        </a:prstGeom>
+      </xdr:spPr>
+      <xdr:style>
+        <a:lnRef idx="3">
+          <a:schemeClr val="dk1"/>
+        </a:lnRef>
+        <a:fillRef idx="0">
+          <a:schemeClr val="dk1"/>
+        </a:fillRef>
+        <a:effectRef idx="2">
+          <a:schemeClr val="dk1"/>
+        </a:effectRef>
+        <a:fontRef idx="minor">
+          <a:schemeClr val="tx1"/>
+        </a:fontRef>
+      </xdr:style>
+      <xdr:txBody>
+        <a:bodyPr vertOverflow="clip" horzOverflow="clip" rtlCol="0" anchor="t"/>
+        <a:lstStyle/>
+        <a:p>
+          <a:pPr algn="l"/>
+          <a:endParaRPr lang="en-GB" sz="1100"/>
+        </a:p>
+      </xdr:txBody>
+    </xdr:sp>
+    <xdr:clientData/>
+  </xdr:twoCellAnchor>
+  <xdr:twoCellAnchor>
+    <xdr:from>
+      <xdr:col>17</xdr:col>
+      <xdr:colOff>352428</xdr:colOff>
+      <xdr:row>29</xdr:row>
+      <xdr:rowOff>47625</xdr:rowOff>
+    </xdr:from>
+    <xdr:to>
+      <xdr:col>23</xdr:col>
+      <xdr:colOff>19051</xdr:colOff>
+      <xdr:row>30</xdr:row>
+      <xdr:rowOff>28575</xdr:rowOff>
+    </xdr:to>
+    <xdr:sp macro="" textlink="">
+      <xdr:nvSpPr>
+        <xdr:cNvPr id="18" name="Left Bracket 17"/>
+        <xdr:cNvSpPr/>
+      </xdr:nvSpPr>
+      <xdr:spPr>
+        <a:xfrm rot="16200000">
+          <a:off x="7900990" y="4576763"/>
+          <a:ext cx="171450" cy="2162173"/>
+        </a:xfrm>
+        <a:prstGeom prst="leftBracket">
+          <a:avLst/>
+        </a:prstGeom>
+      </xdr:spPr>
+      <xdr:style>
+        <a:lnRef idx="3">
+          <a:schemeClr val="dk1"/>
+        </a:lnRef>
+        <a:fillRef idx="0">
+          <a:schemeClr val="dk1"/>
+        </a:fillRef>
+        <a:effectRef idx="2">
+          <a:schemeClr val="dk1"/>
+        </a:effectRef>
+        <a:fontRef idx="minor">
+          <a:schemeClr val="tx1"/>
+        </a:fontRef>
+      </xdr:style>
+      <xdr:txBody>
+        <a:bodyPr vertOverflow="clip" horzOverflow="clip" rtlCol="0" anchor="t"/>
+        <a:lstStyle/>
+        <a:p>
+          <a:pPr algn="l"/>
+          <a:endParaRPr lang="en-GB" sz="1100"/>
+        </a:p>
+      </xdr:txBody>
+    </xdr:sp>
+    <xdr:clientData/>
+  </xdr:twoCellAnchor>
+  <xdr:twoCellAnchor>
+    <xdr:from>
+      <xdr:col>24</xdr:col>
+      <xdr:colOff>9525</xdr:colOff>
+      <xdr:row>29</xdr:row>
+      <xdr:rowOff>9525</xdr:rowOff>
+    </xdr:from>
+    <xdr:to>
+      <xdr:col>24</xdr:col>
+      <xdr:colOff>333375</xdr:colOff>
+      <xdr:row>29</xdr:row>
+      <xdr:rowOff>180975</xdr:rowOff>
+    </xdr:to>
+    <xdr:sp macro="" textlink="">
+      <xdr:nvSpPr>
+        <xdr:cNvPr id="19" name="Left Bracket 18"/>
+        <xdr:cNvSpPr/>
+      </xdr:nvSpPr>
+      <xdr:spPr>
+        <a:xfrm rot="16200000">
+          <a:off x="9505950" y="5457825"/>
+          <a:ext cx="171450" cy="323850"/>
+        </a:xfrm>
+        <a:prstGeom prst="leftBracket">
+          <a:avLst/>
+        </a:prstGeom>
+      </xdr:spPr>
+      <xdr:style>
+        <a:lnRef idx="3">
+          <a:schemeClr val="dk1"/>
+        </a:lnRef>
+        <a:fillRef idx="0">
+          <a:schemeClr val="dk1"/>
+        </a:fillRef>
+        <a:effectRef idx="2">
+          <a:schemeClr val="dk1"/>
+        </a:effectRef>
+        <a:fontRef idx="minor">
+          <a:schemeClr val="tx1"/>
+        </a:fontRef>
+      </xdr:style>
+      <xdr:txBody>
+        <a:bodyPr vertOverflow="clip" horzOverflow="clip" rtlCol="0" anchor="t"/>
+        <a:lstStyle/>
+        <a:p>
+          <a:pPr algn="l"/>
+          <a:endParaRPr lang="en-GB" sz="1100"/>
+        </a:p>
+      </xdr:txBody>
+    </xdr:sp>
+    <xdr:clientData/>
+  </xdr:twoCellAnchor>
+  <xdr:twoCellAnchor>
+    <xdr:from>
+      <xdr:col>18</xdr:col>
+      <xdr:colOff>4</xdr:colOff>
+      <xdr:row>31</xdr:row>
+      <xdr:rowOff>19048</xdr:rowOff>
+    </xdr:from>
+    <xdr:to>
+      <xdr:col>24</xdr:col>
+      <xdr:colOff>323851</xdr:colOff>
+      <xdr:row>32</xdr:row>
+      <xdr:rowOff>47622</xdr:rowOff>
+    </xdr:to>
+    <xdr:sp macro="" textlink="">
+      <xdr:nvSpPr>
+        <xdr:cNvPr id="20" name="Left Bracket 19"/>
+        <xdr:cNvSpPr/>
+      </xdr:nvSpPr>
+      <xdr:spPr>
+        <a:xfrm rot="16200000">
+          <a:off x="8224841" y="4624386"/>
+          <a:ext cx="219074" cy="2819397"/>
+        </a:xfrm>
+        <a:prstGeom prst="leftBracket">
+          <a:avLst/>
+        </a:prstGeom>
+      </xdr:spPr>
+      <xdr:style>
+        <a:lnRef idx="3">
+          <a:schemeClr val="dk1"/>
+        </a:lnRef>
+        <a:fillRef idx="0">
+          <a:schemeClr val="dk1"/>
+        </a:fillRef>
+        <a:effectRef idx="2">
+          <a:schemeClr val="dk1"/>
+        </a:effectRef>
+        <a:fontRef idx="minor">
+          <a:schemeClr val="tx1"/>
+        </a:fontRef>
+      </xdr:style>
+      <xdr:txBody>
+        <a:bodyPr vertOverflow="clip" horzOverflow="clip" rtlCol="0" anchor="t"/>
+        <a:lstStyle/>
+        <a:p>
+          <a:pPr algn="l"/>
+          <a:endParaRPr lang="en-GB" sz="1100"/>
+        </a:p>
+      </xdr:txBody>
+    </xdr:sp>
+    <xdr:clientData/>
+  </xdr:twoCellAnchor>
+  <xdr:twoCellAnchor>
+    <xdr:from>
+      <xdr:col>17</xdr:col>
+      <xdr:colOff>28580</xdr:colOff>
+      <xdr:row>33</xdr:row>
+      <xdr:rowOff>9523</xdr:rowOff>
+    </xdr:from>
+    <xdr:to>
+      <xdr:col>26</xdr:col>
+      <xdr:colOff>3</xdr:colOff>
+      <xdr:row>34</xdr:row>
+      <xdr:rowOff>28576</xdr:rowOff>
+    </xdr:to>
+    <xdr:sp macro="" textlink="">
+      <xdr:nvSpPr>
+        <xdr:cNvPr id="22" name="Left Bracket 21"/>
+        <xdr:cNvSpPr/>
+      </xdr:nvSpPr>
+      <xdr:spPr>
+        <a:xfrm rot="16200000">
+          <a:off x="8267702" y="4610101"/>
+          <a:ext cx="209553" cy="3581398"/>
+        </a:xfrm>
+        <a:prstGeom prst="leftBracket">
+          <a:avLst/>
+        </a:prstGeom>
+      </xdr:spPr>
+      <xdr:style>
+        <a:lnRef idx="3">
+          <a:schemeClr val="dk1"/>
+        </a:lnRef>
+        <a:fillRef idx="0">
+          <a:schemeClr val="dk1"/>
+        </a:fillRef>
+        <a:effectRef idx="2">
+          <a:schemeClr val="dk1"/>
+        </a:effectRef>
+        <a:fontRef idx="minor">
+          <a:schemeClr val="tx1"/>
+        </a:fontRef>
+      </xdr:style>
+      <xdr:txBody>
+        <a:bodyPr vertOverflow="clip" horzOverflow="clip" rtlCol="0" anchor="t"/>
+        <a:lstStyle/>
+        <a:p>
+          <a:pPr algn="l"/>
+          <a:endParaRPr lang="en-GB" sz="1100"/>
+        </a:p>
+      </xdr:txBody>
+    </xdr:sp>
+    <xdr:clientData/>
+  </xdr:twoCellAnchor>
+  <xdr:twoCellAnchor>
+    <xdr:from>
+      <xdr:col>2</xdr:col>
+      <xdr:colOff>361955</xdr:colOff>
+      <xdr:row>35</xdr:row>
+      <xdr:rowOff>9524</xdr:rowOff>
+    </xdr:from>
+    <xdr:to>
+      <xdr:col>25</xdr:col>
+      <xdr:colOff>333378</xdr:colOff>
+      <xdr:row>36</xdr:row>
+      <xdr:rowOff>9526</xdr:rowOff>
+    </xdr:to>
+    <xdr:sp macro="" textlink="">
+      <xdr:nvSpPr>
+        <xdr:cNvPr id="23" name="Left Bracket 22"/>
+        <xdr:cNvSpPr/>
+      </xdr:nvSpPr>
+      <xdr:spPr>
+        <a:xfrm rot="16200000">
+          <a:off x="5638803" y="2381251"/>
+          <a:ext cx="190502" cy="8782048"/>
+        </a:xfrm>
+        <a:prstGeom prst="leftBracket">
+          <a:avLst/>
+        </a:prstGeom>
+      </xdr:spPr>
+      <xdr:style>
+        <a:lnRef idx="3">
+          <a:schemeClr val="dk1"/>
+        </a:lnRef>
+        <a:fillRef idx="0">
+          <a:schemeClr val="dk1"/>
+        </a:fillRef>
+        <a:effectRef idx="2">
+          <a:schemeClr val="dk1"/>
+        </a:effectRef>
+        <a:fontRef idx="minor">
+          <a:schemeClr val="tx1"/>
+        </a:fontRef>
+      </xdr:style>
+      <xdr:txBody>
+        <a:bodyPr vertOverflow="clip" horzOverflow="clip" rtlCol="0" anchor="t"/>
+        <a:lstStyle/>
+        <a:p>
+          <a:pPr algn="l"/>
+          <a:endParaRPr lang="en-GB" sz="1100"/>
+        </a:p>
+      </xdr:txBody>
+    </xdr:sp>
+    <xdr:clientData/>
+  </xdr:twoCellAnchor>
+  <xdr:twoCellAnchor>
+    <xdr:from>
+      <xdr:col>1</xdr:col>
+      <xdr:colOff>9529</xdr:colOff>
+      <xdr:row>36</xdr:row>
+      <xdr:rowOff>180973</xdr:rowOff>
+    </xdr:from>
+    <xdr:to>
+      <xdr:col>26</xdr:col>
+      <xdr:colOff>19049</xdr:colOff>
+      <xdr:row>38</xdr:row>
+      <xdr:rowOff>28574</xdr:rowOff>
+    </xdr:to>
+    <xdr:sp macro="" textlink="">
+      <xdr:nvSpPr>
+        <xdr:cNvPr id="24" name="Left Bracket 23"/>
+        <xdr:cNvSpPr/>
+      </xdr:nvSpPr>
+      <xdr:spPr>
+        <a:xfrm rot="16200000">
+          <a:off x="5286376" y="2371726"/>
+          <a:ext cx="228601" cy="9563095"/>
+        </a:xfrm>
+        <a:prstGeom prst="leftBracket">
+          <a:avLst/>
+        </a:prstGeom>
+      </xdr:spPr>
+      <xdr:style>
+        <a:lnRef idx="3">
+          <a:schemeClr val="dk1"/>
+        </a:lnRef>
+        <a:fillRef idx="0">
+          <a:schemeClr val="dk1"/>
+        </a:fillRef>
+        <a:effectRef idx="2">
+          <a:schemeClr val="dk1"/>
+        </a:effectRef>
+        <a:fontRef idx="minor">
+          <a:schemeClr val="tx1"/>
+        </a:fontRef>
+      </xdr:style>
+      <xdr:txBody>
+        <a:bodyPr vertOverflow="clip" horzOverflow="clip" rtlCol="0" anchor="t"/>
+        <a:lstStyle/>
+        <a:p>
+          <a:pPr algn="l"/>
+          <a:endParaRPr lang="en-GB" sz="1100"/>
+        </a:p>
+      </xdr:txBody>
+    </xdr:sp>
+    <xdr:clientData/>
+  </xdr:twoCellAnchor>
+</xdr:wsDr>
+</file>
+
 <file path=xl/theme/theme1.xml><?xml version="1.0" encoding="utf-8"?>
 <a:theme xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" name="Office Theme">
   <a:themeElements>
@@ -1245,25 +2358,25 @@
 
 <file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="B2:Z11"/>
+  <dimension ref="A2:AA53"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="B6" sqref="B6:B12"/>
+    <sheetView tabSelected="1" topLeftCell="A12" zoomScale="90" zoomScaleNormal="90" workbookViewId="0">
+      <selection activeCell="C46" sqref="C46:D48"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15"/>
   <cols>
-    <col min="2" max="18" width="5.5703125" customWidth="1"/>
-    <col min="19" max="19" width="9.5703125" bestFit="1" customWidth="1"/>
-    <col min="20" max="27" width="5.5703125" customWidth="1"/>
+    <col min="2" max="19" width="5.5703125" customWidth="1"/>
+    <col min="20" max="20" width="9.5703125" bestFit="1" customWidth="1"/>
+    <col min="21" max="27" width="5.5703125" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="2" spans="2:26">
+    <row r="2" spans="2:27">
       <c r="B2" t="s">
         <v>51</v>
       </c>
     </row>
-    <row r="3" spans="2:26" s="1" customFormat="1">
+    <row r="3" spans="2:27" s="1" customFormat="1">
       <c r="B3" s="1" t="s">
         <v>52</v>
       </c>
@@ -1316,61 +2429,434 @@
         <v>62</v>
       </c>
       <c r="S3" s="1" t="s">
+        <v>62</v>
+      </c>
+      <c r="T3" s="1" t="s">
         <v>63</v>
       </c>
-      <c r="T3" s="1" t="s">
+      <c r="U3" s="1" t="s">
         <v>64</v>
       </c>
-      <c r="U3" s="1" t="s">
+      <c r="V3" s="1" t="s">
         <v>65</v>
       </c>
-      <c r="V3" s="1" t="s">
+      <c r="W3" s="1" t="s">
         <v>56</v>
       </c>
-      <c r="W3" s="1" t="s">
+      <c r="X3" s="1" t="s">
         <v>66</v>
       </c>
-      <c r="X3" s="1" t="s">
+      <c r="Y3" s="1" t="s">
         <v>60</v>
       </c>
-      <c r="Y3" s="1" t="s">
+      <c r="Z3" s="1" t="s">
         <v>65</v>
       </c>
-      <c r="Z3" s="1" t="s">
+      <c r="AA3" s="1" t="s">
         <v>67</v>
       </c>
     </row>
-    <row r="6" spans="2:26">
+    <row r="6" spans="2:27">
       <c r="B6" t="s">
         <v>68</v>
       </c>
     </row>
-    <row r="7" spans="2:26">
+    <row r="7" spans="2:27">
       <c r="B7" t="s">
         <v>69</v>
       </c>
     </row>
-    <row r="8" spans="2:26">
+    <row r="8" spans="2:27">
       <c r="B8" t="s">
         <v>70</v>
       </c>
     </row>
-    <row r="9" spans="2:26">
+    <row r="9" spans="2:27">
       <c r="B9" t="s">
         <v>71</v>
       </c>
     </row>
-    <row r="10" spans="2:26">
+    <row r="10" spans="2:27">
       <c r="B10" t="s">
         <v>72</v>
       </c>
     </row>
-    <row r="11" spans="2:26">
+    <row r="11" spans="2:27">
       <c r="B11" t="s">
         <v>73</v>
       </c>
     </row>
+    <row r="15" spans="2:27" s="1" customFormat="1">
+      <c r="B15" s="1" t="s">
+        <v>52</v>
+      </c>
+      <c r="C15" s="1" t="s">
+        <v>53</v>
+      </c>
+      <c r="D15" s="1" t="s">
+        <v>54</v>
+      </c>
+      <c r="E15" s="1" t="s">
+        <v>55</v>
+      </c>
+      <c r="F15" s="1" t="s">
+        <v>56</v>
+      </c>
+      <c r="G15" s="1" t="s">
+        <v>57</v>
+      </c>
+      <c r="H15" s="1" t="s">
+        <v>58</v>
+      </c>
+      <c r="I15" s="1" t="s">
+        <v>54</v>
+      </c>
+      <c r="J15" s="1" t="s">
+        <v>59</v>
+      </c>
+      <c r="K15" s="1" t="s">
+        <v>56</v>
+      </c>
+      <c r="L15" s="1" t="s">
+        <v>59</v>
+      </c>
+      <c r="M15" s="1">
+        <v>100</v>
+      </c>
+      <c r="N15" s="1" t="s">
+        <v>57</v>
+      </c>
+      <c r="O15" s="1" t="s">
+        <v>60</v>
+      </c>
+      <c r="P15" s="1" t="s">
+        <v>61</v>
+      </c>
+      <c r="Q15" s="1" t="s">
+        <v>57</v>
+      </c>
+      <c r="R15" s="1" t="s">
+        <v>62</v>
+      </c>
+      <c r="S15" s="1" t="s">
+        <v>62</v>
+      </c>
+      <c r="T15" s="1" t="s">
+        <v>63</v>
+      </c>
+      <c r="U15" s="1" t="s">
+        <v>64</v>
+      </c>
+      <c r="V15" s="1" t="s">
+        <v>65</v>
+      </c>
+      <c r="W15" s="1" t="s">
+        <v>56</v>
+      </c>
+      <c r="X15" s="1" t="s">
+        <v>66</v>
+      </c>
+      <c r="Y15" s="1" t="s">
+        <v>60</v>
+      </c>
+      <c r="Z15" s="1" t="s">
+        <v>65</v>
+      </c>
+      <c r="AA15" s="1" t="s">
+        <v>67</v>
+      </c>
+    </row>
+    <row r="16" spans="2:27" s="1" customFormat="1">
+      <c r="B16" s="1">
+        <v>1</v>
+      </c>
+      <c r="D16" s="1">
+        <v>2</v>
+      </c>
+      <c r="F16" s="1">
+        <v>3</v>
+      </c>
+    </row>
+    <row r="17" spans="4:25" s="1" customFormat="1"/>
+    <row r="18" spans="4:25" s="1" customFormat="1">
+      <c r="D18" s="1">
+        <v>4</v>
+      </c>
+      <c r="I18" s="1">
+        <v>5</v>
+      </c>
+      <c r="K18" s="1">
+        <v>6</v>
+      </c>
+    </row>
+    <row r="19" spans="4:25" s="1" customFormat="1"/>
+    <row r="20" spans="4:25" s="1" customFormat="1">
+      <c r="I20" s="1">
+        <v>7</v>
+      </c>
+      <c r="M20" s="1">
+        <v>8</v>
+      </c>
+      <c r="O20" s="1">
+        <v>9</v>
+      </c>
+    </row>
+    <row r="21" spans="4:25" s="1" customFormat="1"/>
+    <row r="22" spans="4:25" s="1" customFormat="1">
+      <c r="M22" s="1">
+        <v>10</v>
+      </c>
+    </row>
+    <row r="23" spans="4:25" s="1" customFormat="1"/>
+    <row r="24" spans="4:25" s="1" customFormat="1">
+      <c r="I24" s="1">
+        <v>11</v>
+      </c>
+    </row>
+    <row r="25" spans="4:25" s="1" customFormat="1"/>
+    <row r="26" spans="4:25" s="1" customFormat="1">
+      <c r="H26" s="1">
+        <v>12</v>
+      </c>
+    </row>
+    <row r="27" spans="4:25" s="1" customFormat="1"/>
+    <row r="28" spans="4:25" s="1" customFormat="1">
+      <c r="D28" s="1">
+        <v>13</v>
+      </c>
+      <c r="W28" s="1">
+        <v>14</v>
+      </c>
+    </row>
+    <row r="29" spans="4:25" s="1" customFormat="1"/>
+    <row r="30" spans="4:25" s="1" customFormat="1">
+      <c r="S30" s="1">
+        <v>15</v>
+      </c>
+      <c r="Y30" s="1">
+        <v>16</v>
+      </c>
+    </row>
+    <row r="31" spans="4:25" s="1" customFormat="1"/>
+    <row r="32" spans="4:25" s="1" customFormat="1">
+      <c r="S32" s="1">
+        <v>17</v>
+      </c>
+    </row>
+    <row r="33" spans="1:21" s="1" customFormat="1"/>
+    <row r="34" spans="1:21" s="1" customFormat="1">
+      <c r="R34" s="1">
+        <v>18</v>
+      </c>
+    </row>
+    <row r="35" spans="1:21" s="1" customFormat="1"/>
+    <row r="36" spans="1:21" s="1" customFormat="1">
+      <c r="D36" s="1">
+        <v>19</v>
+      </c>
+    </row>
+    <row r="37" spans="1:21" s="1" customFormat="1"/>
+    <row r="38" spans="1:21" s="1" customFormat="1">
+      <c r="B38" s="1">
+        <v>20</v>
+      </c>
+    </row>
+    <row r="39" spans="1:21" s="1" customFormat="1"/>
+    <row r="43" spans="1:21">
+      <c r="B43">
+        <v>1</v>
+      </c>
+      <c r="C43">
+        <v>2</v>
+      </c>
+      <c r="D43">
+        <v>3</v>
+      </c>
+      <c r="E43">
+        <v>4</v>
+      </c>
+      <c r="F43">
+        <v>5</v>
+      </c>
+      <c r="G43">
+        <v>6</v>
+      </c>
+      <c r="H43">
+        <v>7</v>
+      </c>
+      <c r="I43">
+        <v>8</v>
+      </c>
+      <c r="J43">
+        <v>9</v>
+      </c>
+      <c r="K43">
+        <v>10</v>
+      </c>
+      <c r="L43">
+        <v>11</v>
+      </c>
+      <c r="M43">
+        <v>12</v>
+      </c>
+      <c r="N43">
+        <v>13</v>
+      </c>
+      <c r="O43">
+        <v>14</v>
+      </c>
+      <c r="P43">
+        <v>15</v>
+      </c>
+      <c r="Q43">
+        <v>16</v>
+      </c>
+      <c r="R43">
+        <v>17</v>
+      </c>
+      <c r="S43">
+        <v>18</v>
+      </c>
+      <c r="T43">
+        <v>19</v>
+      </c>
+      <c r="U43">
+        <v>20</v>
+      </c>
+    </row>
+    <row r="44" spans="1:21">
+      <c r="A44" t="s">
+        <v>74</v>
+      </c>
+      <c r="B44" t="s">
+        <v>75</v>
+      </c>
+      <c r="U44" s="3" t="s">
+        <v>93</v>
+      </c>
+    </row>
+    <row r="45" spans="1:21">
+      <c r="B45" t="s">
+        <v>76</v>
+      </c>
+    </row>
+    <row r="46" spans="1:21">
+      <c r="C46" t="s">
+        <v>60</v>
+      </c>
+      <c r="E46" s="3" t="s">
+        <v>78</v>
+      </c>
+      <c r="N46" s="3" t="s">
+        <v>86</v>
+      </c>
+      <c r="T46" s="3" t="s">
+        <v>92</v>
+      </c>
+    </row>
+    <row r="47" spans="1:21">
+      <c r="D47" t="s">
+        <v>80</v>
+      </c>
+      <c r="E47" t="s">
+        <v>81</v>
+      </c>
+      <c r="N47" t="s">
+        <v>81</v>
+      </c>
+    </row>
+    <row r="48" spans="1:21">
+      <c r="D48" t="s">
+        <v>77</v>
+      </c>
+      <c r="F48" t="s">
+        <v>58</v>
+      </c>
+      <c r="M48" s="3" t="s">
+        <v>85</v>
+      </c>
+      <c r="N48" t="s">
+        <v>58</v>
+      </c>
+      <c r="S48" s="3" t="s">
+        <v>91</v>
+      </c>
+    </row>
+    <row r="49" spans="6:18">
+      <c r="F49" t="s">
+        <v>60</v>
+      </c>
+      <c r="H49" s="3" t="s">
+        <v>79</v>
+      </c>
+      <c r="L49" s="3" t="s">
+        <v>84</v>
+      </c>
+      <c r="N49" t="s">
+        <v>58</v>
+      </c>
+      <c r="P49" s="3" t="s">
+        <v>89</v>
+      </c>
+      <c r="R49" s="3" t="s">
+        <v>90</v>
+      </c>
+    </row>
+    <row r="50" spans="6:18">
+      <c r="G50" s="2" t="s">
+        <v>82</v>
+      </c>
+      <c r="H50" s="2" t="s">
+        <v>82</v>
+      </c>
+      <c r="L50" t="s">
+        <v>65</v>
+      </c>
+      <c r="N50" t="s">
+        <v>87</v>
+      </c>
+      <c r="P50" t="s">
+        <v>88</v>
+      </c>
+      <c r="R50" t="s">
+        <v>65</v>
+      </c>
+    </row>
+    <row r="51" spans="6:18">
+      <c r="G51" t="s">
+        <v>77</v>
+      </c>
+      <c r="I51">
+        <v>100</v>
+      </c>
+      <c r="K51" s="3" t="s">
+        <v>83</v>
+      </c>
+      <c r="N51" t="s">
+        <v>64</v>
+      </c>
+      <c r="Q51" t="s">
+        <v>60</v>
+      </c>
+    </row>
+    <row r="52" spans="6:18">
+      <c r="J52" t="s">
+        <v>81</v>
+      </c>
+      <c r="N52" t="s">
+        <v>65</v>
+      </c>
+    </row>
+    <row r="53" spans="6:18">
+      <c r="J53" t="s">
+        <v>60</v>
+      </c>
+      <c r="O53" t="s">
+        <v>77</v>
+      </c>
+    </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+  <drawing r:id="rId1"/>
 </worksheet>
 </file>
</xml_diff>